<commit_message>
A few more updates.
</commit_message>
<xml_diff>
--- a/doc/WorkingDrafts/Components.xlsx
+++ b/doc/WorkingDrafts/Components.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>SST core</t>
   </si>
@@ -36,15 +36,6 @@
     <t>scheduler</t>
   </si>
   <si>
-    <t>McPAT</t>
-  </si>
-  <si>
-    <t>ORION</t>
-  </si>
-  <si>
-    <t>HotSpot</t>
-  </si>
-  <si>
     <t>DRAMSimTrace</t>
   </si>
   <si>
@@ -102,15 +93,9 @@
     <t>http://www.pdl.cmu.edu/DiskSim/</t>
   </si>
   <si>
-    <t>http://www.pdl.cmu.edu/DiskSim/#code</t>
-  </si>
-  <si>
     <t>[sst]disksim</t>
   </si>
   <si>
-    <t>IntSim</t>
-  </si>
-  <si>
     <t>http://www.hpl.hp.com/research/mcpat/</t>
   </si>
   <si>
@@ -120,7 +105,28 @@
     <t>a glue directory in sst directory</t>
   </si>
   <si>
-    <t>sent email to Genie</t>
+    <t>Iris</t>
+  </si>
+  <si>
+    <t>http://projects.csail.mit.edu/cgi-bin/wiki/view/LSPgroup/OrionPage</t>
+  </si>
+  <si>
+    <t>http://deepaksekar.weebly.com/intsim.html</t>
+  </si>
+  <si>
+    <t>http://lava.cs.virginia.edu/HotSpot/documentation.htm</t>
+  </si>
+  <si>
+    <t>McPAT v0.7</t>
+  </si>
+  <si>
+    <t>ORION v2.0 (May 2009)</t>
+  </si>
+  <si>
+    <t>IntSim V1.0</t>
+  </si>
+  <si>
+    <t>HotSpot v5.0</t>
   </si>
 </sst>
 </file>
@@ -479,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,16 +501,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
         <v>11</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -512,10 +518,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -523,44 +529,42 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>28</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -572,10 +576,10 @@
         <v>3</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -583,10 +587,10 @@
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -594,64 +598,69 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="C13" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -667,17 +676,19 @@
     <hyperlink ref="B8" r:id="rId9"/>
     <hyperlink ref="C8" r:id="rId10"/>
     <hyperlink ref="B6" r:id="rId11"/>
-    <hyperlink ref="C6" r:id="rId12" location="code"/>
-    <hyperlink ref="C10" r:id="rId13"/>
-    <hyperlink ref="C11" r:id="rId14"/>
-    <hyperlink ref="C12" r:id="rId15"/>
-    <hyperlink ref="C13" r:id="rId16"/>
-    <hyperlink ref="C14" r:id="rId17"/>
-    <hyperlink ref="B11" r:id="rId18"/>
-    <hyperlink ref="C5" r:id="rId19"/>
+    <hyperlink ref="C10" r:id="rId12"/>
+    <hyperlink ref="C11" r:id="rId13"/>
+    <hyperlink ref="C12" r:id="rId14"/>
+    <hyperlink ref="C13" r:id="rId15"/>
+    <hyperlink ref="C14" r:id="rId16"/>
+    <hyperlink ref="B11" r:id="rId17"/>
+    <hyperlink ref="C5" r:id="rId18"/>
+    <hyperlink ref="B12" r:id="rId19"/>
+    <hyperlink ref="B13" r:id="rId20"/>
+    <hyperlink ref="B14" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId20"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
 

</xml_diff>